<commit_message>
Ajustes a las mediciones de performances segun ultimos cambios
</commit_message>
<xml_diff>
--- a/Documentacion/drafts/20120604/Comparacion de performance en envio y recepcion simple.xlsx
+++ b/Documentacion/drafts/20120604/Comparacion de performance en envio y recepcion simple.xlsx
@@ -339,10 +339,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>21553.981861</c:v>
+                  <c:v>12137.010151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4639.5139721696178</c:v>
+                  <c:v>8239.2614619145497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -385,11 +385,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="159038080"/>
-        <c:axId val="159048064"/>
+        <c:axId val="157923968"/>
+        <c:axId val="157933952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="159038080"/>
+        <c:axId val="157923968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,7 +398,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159048064"/>
+        <c:crossAx val="157933952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -406,7 +406,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159048064"/>
+        <c:axId val="157933952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -417,7 +417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159038080"/>
+        <c:crossAx val="157923968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -541,10 +541,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>21553.981861</c:v>
+                  <c:v>12137.010151</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4639.5139721696178</c:v>
+                  <c:v>8239.2614619145497</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -559,11 +559,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="159339264"/>
-        <c:axId val="159340800"/>
+        <c:axId val="158225152"/>
+        <c:axId val="158226688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="159339264"/>
+        <c:axId val="158225152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159340800"/>
+        <c:crossAx val="158226688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -580,7 +580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="159340800"/>
+        <c:axId val="158226688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -591,7 +591,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159339264"/>
+        <c:crossAx val="158225152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -969,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:G62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1217,18 +1217,18 @@
         <v>100000</v>
       </c>
       <c r="D21">
-        <v>36669.51498</v>
+        <v>4222.4483840000003</v>
       </c>
       <c r="E21">
         <f>1000*C21/D21</f>
-        <v>2727.0608857123202</v>
+        <v>23682.941958255087</v>
       </c>
       <c r="F21">
         <f>D21/C21</f>
-        <v>0.36669514980000001</v>
+        <v>4.222448384E-2</v>
       </c>
       <c r="G21">
-        <v>24005.0801695962</v>
+        <v>10.117475170000001</v>
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
@@ -1236,18 +1236,18 @@
         <v>10000</v>
       </c>
       <c r="D22">
-        <v>943.49672899999996</v>
+        <v>452.89974000000001</v>
       </c>
       <c r="E22">
         <f>1000*C22/D22</f>
-        <v>10598.870873244967</v>
+        <v>22079.942019838651</v>
       </c>
       <c r="F22">
         <f>D22/C22</f>
-        <v>9.4349672900000001E-2</v>
+        <v>4.5289974000000004E-2</v>
       </c>
       <c r="G22">
-        <v>371.70964882669898</v>
+        <v>9.5499764860000003</v>
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
@@ -1255,18 +1255,18 @@
         <v>1000</v>
       </c>
       <c r="D23">
-        <v>201.97874300000001</v>
+        <v>98.912851000000003</v>
       </c>
       <c r="E23">
         <f>1000*C23/D23</f>
-        <v>4951.0160581601403</v>
+        <v>10109.90978310796</v>
       </c>
       <c r="F23">
         <f>D23/C23</f>
-        <v>0.20197874300000002</v>
+        <v>9.891285100000001E-2</v>
       </c>
       <c r="G23">
-        <v>70.656949707999999</v>
+        <v>7.3004350889999996</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
@@ -1304,18 +1304,18 @@
         <v>100000</v>
       </c>
       <c r="D29">
-        <v>21553.981861</v>
+        <v>12137.010151</v>
       </c>
       <c r="E29">
         <f>1000*C29/D29</f>
-        <v>4639.5139721696178</v>
+        <v>8239.2614619145497</v>
       </c>
       <c r="F29">
         <f>D29/C29</f>
-        <v>0.21553981860999999</v>
+        <v>0.12137010151000001</v>
       </c>
       <c r="G29">
-        <v>15673.7990884315</v>
+        <v>1834.5638976170601</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
@@ -1323,18 +1323,18 @@
         <v>10000</v>
       </c>
       <c r="D30">
-        <v>1827.530874</v>
+        <v>1583.176633</v>
       </c>
       <c r="E30">
         <f>1000*C30/D30</f>
-        <v>5471.8637820397225</v>
+        <v>6316.4146005937164</v>
       </c>
       <c r="F30">
         <f>D30/C30</f>
-        <v>0.18275308740000001</v>
+        <v>0.15831766329999999</v>
       </c>
       <c r="G30">
-        <v>1190.8694713624</v>
+        <v>268.70276339669999</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
@@ -1342,18 +1342,18 @@
         <v>1000</v>
       </c>
       <c r="D31">
-        <v>327.243267</v>
+        <v>394.179149</v>
       </c>
       <c r="E31">
         <f>1000*C31/D31</f>
-        <v>3055.8306337896329</v>
+        <v>2536.9175476098053</v>
       </c>
       <c r="F31">
         <f>D31/C31</f>
-        <v>0.327243267</v>
+        <v>0.39417914900000001</v>
       </c>
       <c r="G31">
-        <v>113.376419614</v>
+        <v>181.454856963</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">

</xml_diff>